<commit_message>
successfully created the regression script
</commit_message>
<xml_diff>
--- a/Early_Stage_quarterly_average.xlsx
+++ b/Early_Stage_quarterly_average.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Announced Date</t>
+  </si>
+  <si>
+    <t>Money Raised Currency (in USD)</t>
   </si>
   <si>
     <t>2007Q1</t>
@@ -579,525 +582,525 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>0</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2412937</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>3</v>
       </c>
       <c r="B3">
         <v>2516458</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>4</v>
       </c>
       <c r="B4">
         <v>2475597</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>5</v>
       </c>
       <c r="B5">
         <v>2844712</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>6</v>
       </c>
       <c r="B6">
         <v>2575179</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>7</v>
       </c>
       <c r="B7">
         <v>2376245</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>8</v>
       </c>
       <c r="B8">
         <v>2737144</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1999052</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>10</v>
       </c>
       <c r="B10">
         <v>2473886</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>11</v>
       </c>
       <c r="B11">
         <v>2015864</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>12</v>
       </c>
       <c r="B12">
         <v>1997574</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
+      <c r="A13" t="s">
+        <v>13</v>
       </c>
       <c r="B13">
         <v>2430146</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
+      <c r="A14" t="s">
+        <v>14</v>
       </c>
       <c r="B14">
         <v>2046462</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>15</v>
       </c>
       <c r="B15">
         <v>2087183</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>16</v>
       </c>
       <c r="B16">
         <v>2083342</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
+      <c r="A17" t="s">
+        <v>17</v>
       </c>
       <c r="B17">
         <v>1923746</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
+      <c r="A18" t="s">
+        <v>18</v>
       </c>
       <c r="B18">
         <v>2108615</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
+      <c r="A19" t="s">
+        <v>19</v>
       </c>
       <c r="B19">
         <v>2484657</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
+      <c r="A20" t="s">
+        <v>20</v>
       </c>
       <c r="B20">
         <v>2137694</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
+      <c r="A21" t="s">
+        <v>21</v>
       </c>
       <c r="B21">
         <v>2888389</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
+      <c r="A22" t="s">
+        <v>22</v>
       </c>
       <c r="B22">
         <v>2648436</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
+      <c r="A23" t="s">
+        <v>23</v>
       </c>
       <c r="B23">
         <v>2063542</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
+      <c r="A24" t="s">
+        <v>24</v>
       </c>
       <c r="B24">
         <v>2223340</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
+      <c r="A25" t="s">
+        <v>25</v>
       </c>
       <c r="B25">
         <v>2484178</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
+      <c r="A26" t="s">
+        <v>26</v>
       </c>
       <c r="B26">
         <v>2875075</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
+      <c r="A27" t="s">
+        <v>27</v>
       </c>
       <c r="B27">
         <v>3528236</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
+      <c r="A28" t="s">
+        <v>28</v>
       </c>
       <c r="B28">
         <v>2316190</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
+      <c r="A29" t="s">
+        <v>29</v>
       </c>
       <c r="B29">
         <v>2906941</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
-        <v>29</v>
+      <c r="A30" t="s">
+        <v>30</v>
       </c>
       <c r="B30">
         <v>2718062</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
+      <c r="A31" t="s">
+        <v>31</v>
       </c>
       <c r="B31">
         <v>3341233</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
+      <c r="A32" t="s">
+        <v>32</v>
       </c>
       <c r="B32">
         <v>2886392</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
-        <v>32</v>
+      <c r="A33" t="s">
+        <v>33</v>
       </c>
       <c r="B33">
         <v>2924041</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
+      <c r="A34" t="s">
+        <v>34</v>
       </c>
       <c r="B34">
         <v>2981908</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
+      <c r="A35" t="s">
+        <v>35</v>
       </c>
       <c r="B35">
         <v>3973301</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
+      <c r="A36" t="s">
+        <v>36</v>
       </c>
       <c r="B36">
         <v>3615799</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
+      <c r="A37" t="s">
+        <v>37</v>
       </c>
       <c r="B37">
         <v>3729135</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
+      <c r="A38" t="s">
+        <v>38</v>
       </c>
       <c r="B38">
         <v>3859115</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
+      <c r="A39" t="s">
+        <v>39</v>
       </c>
       <c r="B39">
         <v>3785235</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
+      <c r="A40" t="s">
+        <v>40</v>
       </c>
       <c r="B40">
         <v>3478265</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
-        <v>40</v>
+      <c r="A41" t="s">
+        <v>41</v>
       </c>
       <c r="B41">
         <v>4130019</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
+      <c r="A42" t="s">
+        <v>42</v>
       </c>
       <c r="B42">
         <v>4023013</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
+      <c r="A43" t="s">
+        <v>43</v>
       </c>
       <c r="B43">
         <v>3834902</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
+      <c r="A44" t="s">
+        <v>44</v>
       </c>
       <c r="B44">
         <v>4142582</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="1" t="s">
-        <v>44</v>
+      <c r="A45" t="s">
+        <v>45</v>
       </c>
       <c r="B45">
         <v>4082293</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="1" t="s">
-        <v>45</v>
+      <c r="A46" t="s">
+        <v>46</v>
       </c>
       <c r="B46">
         <v>5381185</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="1" t="s">
-        <v>46</v>
+      <c r="A47" t="s">
+        <v>47</v>
       </c>
       <c r="B47">
         <v>4737539</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="1" t="s">
-        <v>47</v>
+      <c r="A48" t="s">
+        <v>48</v>
       </c>
       <c r="B48">
         <v>4736823</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="1" t="s">
-        <v>48</v>
+      <c r="A49" t="s">
+        <v>49</v>
       </c>
       <c r="B49">
         <v>5446476</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="1" t="s">
-        <v>49</v>
+      <c r="A50" t="s">
+        <v>50</v>
       </c>
       <c r="B50">
         <v>5584087</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="1" t="s">
-        <v>50</v>
+      <c r="A51" t="s">
+        <v>51</v>
       </c>
       <c r="B51">
         <v>5131187</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="1" t="s">
-        <v>51</v>
+      <c r="A52" t="s">
+        <v>52</v>
       </c>
       <c r="B52">
         <v>5683340</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="1" t="s">
-        <v>52</v>
+      <c r="A53" t="s">
+        <v>53</v>
       </c>
       <c r="B53">
         <v>5786176</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="1" t="s">
-        <v>53</v>
+      <c r="A54" t="s">
+        <v>54</v>
       </c>
       <c r="B54">
         <v>5064241</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="1" t="s">
-        <v>54</v>
+      <c r="A55" t="s">
+        <v>55</v>
       </c>
       <c r="B55">
         <v>6725769</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="1" t="s">
-        <v>55</v>
+      <c r="A56" t="s">
+        <v>56</v>
       </c>
       <c r="B56">
         <v>5325289</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="1" t="s">
-        <v>56</v>
+      <c r="A57" t="s">
+        <v>57</v>
       </c>
       <c r="B57">
         <v>7447459</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="1" t="s">
-        <v>57</v>
+      <c r="A58" t="s">
+        <v>58</v>
       </c>
       <c r="B58">
         <v>9533346</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="1" t="s">
-        <v>58</v>
+      <c r="A59" t="s">
+        <v>59</v>
       </c>
       <c r="B59">
         <v>8657778</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="1" t="s">
-        <v>59</v>
+      <c r="A60" t="s">
+        <v>60</v>
       </c>
       <c r="B60">
         <v>8461372</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="1" t="s">
-        <v>60</v>
+      <c r="A61" t="s">
+        <v>61</v>
       </c>
       <c r="B61">
         <v>10285148</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="1" t="s">
-        <v>61</v>
+      <c r="A62" t="s">
+        <v>62</v>
       </c>
       <c r="B62">
         <v>8685272</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="1" t="s">
-        <v>62</v>
+      <c r="A63" t="s">
+        <v>63</v>
       </c>
       <c r="B63">
         <v>7859784</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="1" t="s">
-        <v>63</v>
+      <c r="A64" t="s">
+        <v>64</v>
       </c>
       <c r="B64">
         <v>9351143</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="1" t="s">
-        <v>64</v>
+      <c r="A65" t="s">
+        <v>65</v>
       </c>
       <c r="B65">
         <v>8024962</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="1" t="s">
-        <v>65</v>
+      <c r="A66" t="s">
+        <v>66</v>
       </c>
       <c r="B66">
         <v>8411099</v>

</xml_diff>